<commit_message>
Automatyczna aktualizacja danych XLSX
</commit_message>
<xml_diff>
--- a/plik_z_danymi.xlsx
+++ b/plik_z_danymi.xlsx
@@ -11,15 +11,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>xd</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -38,9 +47,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -261,7 +273,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>